<commit_message>
Modified MIDI Note Number format
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -58,390 +58,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>000:C-2</t>
-  </si>
-  <si>
-    <t>001:C#-2</t>
-  </si>
-  <si>
-    <t>002:D-2</t>
-  </si>
-  <si>
-    <t>003:D#-2</t>
-  </si>
-  <si>
-    <t>004:E-2</t>
-  </si>
-  <si>
-    <t>005:F-2</t>
-  </si>
-  <si>
-    <t>006:F#-2</t>
-  </si>
-  <si>
-    <t>007:G-2</t>
-  </si>
-  <si>
-    <t>008:G#-2</t>
-  </si>
-  <si>
-    <t>009:A-2</t>
-  </si>
-  <si>
-    <t>010:A#-2</t>
-  </si>
-  <si>
-    <t>011:B-2</t>
-  </si>
-  <si>
-    <t>012:C-1</t>
-  </si>
-  <si>
-    <t>013:C#-1</t>
-  </si>
-  <si>
-    <t>014:D-1</t>
-  </si>
-  <si>
-    <t>015:D#-1</t>
-  </si>
-  <si>
-    <t>016:E-1</t>
-  </si>
-  <si>
-    <t>017:F-1</t>
-  </si>
-  <si>
-    <t>018:F#-1</t>
-  </si>
-  <si>
-    <t>019:G-1</t>
-  </si>
-  <si>
-    <t>020:G#-1</t>
-  </si>
-  <si>
-    <t>021:A-1</t>
-  </si>
-  <si>
-    <t>022:A#-1</t>
-  </si>
-  <si>
-    <t>023:B-1</t>
-  </si>
-  <si>
-    <t>024:C0</t>
-  </si>
-  <si>
-    <t>025:C#0</t>
-  </si>
-  <si>
-    <t>026:D0</t>
-  </si>
-  <si>
-    <t>027:D#0</t>
-  </si>
-  <si>
-    <t>028:E0</t>
-  </si>
-  <si>
-    <t>029:F0</t>
-  </si>
-  <si>
-    <t>030:F#0</t>
-  </si>
-  <si>
-    <t>031:G0</t>
-  </si>
-  <si>
-    <t>032:G#0</t>
-  </si>
-  <si>
-    <t>033:A0</t>
-  </si>
-  <si>
-    <t>034:A#0</t>
-  </si>
-  <si>
-    <t>035:B0</t>
-  </si>
-  <si>
-    <t>036:C1</t>
-  </si>
-  <si>
-    <t>037:C#1</t>
-  </si>
-  <si>
-    <t>038:D1</t>
-  </si>
-  <si>
-    <t>039:D#1</t>
-  </si>
-  <si>
-    <t>040:E1</t>
-  </si>
-  <si>
-    <t>041:F1</t>
-  </si>
-  <si>
-    <t>042:F#1</t>
-  </si>
-  <si>
-    <t>043:G1</t>
-  </si>
-  <si>
-    <t>044:G#1</t>
-  </si>
-  <si>
-    <t>045:A1</t>
-  </si>
-  <si>
-    <t>046:A#1</t>
-  </si>
-  <si>
-    <t>047:B1</t>
-  </si>
-  <si>
-    <t>048:C2</t>
-  </si>
-  <si>
-    <t>049:C#2</t>
-  </si>
-  <si>
-    <t>050:D2</t>
-  </si>
-  <si>
-    <t>051:D#2</t>
-  </si>
-  <si>
-    <t>052:E2</t>
-  </si>
-  <si>
-    <t>053:F2</t>
-  </si>
-  <si>
-    <t>054:F#2</t>
-  </si>
-  <si>
-    <t>055:G2</t>
-  </si>
-  <si>
-    <t>056:G#2</t>
-  </si>
-  <si>
-    <t>057:A2</t>
-  </si>
-  <si>
-    <t>058:A#2</t>
-  </si>
-  <si>
-    <t>059:B2</t>
-  </si>
-  <si>
-    <t>060:C3</t>
-  </si>
-  <si>
-    <t>061:C#3</t>
-  </si>
-  <si>
-    <t>062:D3</t>
-  </si>
-  <si>
-    <t>063:D#3</t>
-  </si>
-  <si>
-    <t>064:E3</t>
-  </si>
-  <si>
-    <t>065:F3</t>
-  </si>
-  <si>
-    <t>066:F#3</t>
-  </si>
-  <si>
-    <t>067:G3</t>
-  </si>
-  <si>
-    <t>068:G#3</t>
-  </si>
-  <si>
-    <t>069:A3</t>
-  </si>
-  <si>
-    <t>070:A#3</t>
-  </si>
-  <si>
-    <t>071:B3</t>
-  </si>
-  <si>
-    <t>072:C4</t>
-  </si>
-  <si>
-    <t>073:C#4</t>
-  </si>
-  <si>
-    <t>074:D4</t>
-  </si>
-  <si>
-    <t>075:D#4</t>
-  </si>
-  <si>
-    <t>076:E4</t>
-  </si>
-  <si>
-    <t>077:F4</t>
-  </si>
-  <si>
-    <t>078:F#4</t>
-  </si>
-  <si>
-    <t>079:G4</t>
-  </si>
-  <si>
-    <t>080:G#4</t>
-  </si>
-  <si>
-    <t>081:A4</t>
-  </si>
-  <si>
-    <t>082:A#4</t>
-  </si>
-  <si>
-    <t>083:B4</t>
-  </si>
-  <si>
-    <t>084:C5</t>
-  </si>
-  <si>
-    <t>085:C#5</t>
-  </si>
-  <si>
-    <t>086:D5</t>
-  </si>
-  <si>
-    <t>087:D#5</t>
-  </si>
-  <si>
-    <t>088:E5</t>
-  </si>
-  <si>
-    <t>089:F5</t>
-  </si>
-  <si>
-    <t>090:F#5</t>
-  </si>
-  <si>
-    <t>091:G5</t>
-  </si>
-  <si>
-    <t>092:G#5</t>
-  </si>
-  <si>
-    <t>093:A5</t>
-  </si>
-  <si>
-    <t>094:A#5</t>
-  </si>
-  <si>
-    <t>095:B5</t>
-  </si>
-  <si>
-    <t>096:C6</t>
-  </si>
-  <si>
-    <t>097:C#6</t>
-  </si>
-  <si>
-    <t>098:D6</t>
-  </si>
-  <si>
-    <t>099:D#6</t>
-  </si>
-  <si>
-    <t>100:E6</t>
-  </si>
-  <si>
-    <t>101:F6</t>
-  </si>
-  <si>
-    <t>102:F#6</t>
-  </si>
-  <si>
-    <t>103:G6</t>
-  </si>
-  <si>
-    <t>104:G#6</t>
-  </si>
-  <si>
-    <t>105:A6</t>
-  </si>
-  <si>
-    <t>106:A#6</t>
-  </si>
-  <si>
-    <t>107:B6</t>
-  </si>
-  <si>
-    <t>108:C7</t>
-  </si>
-  <si>
-    <t>109:C#7</t>
-  </si>
-  <si>
-    <t>110:D7</t>
-  </si>
-  <si>
-    <t>111:D#7</t>
-  </si>
-  <si>
-    <t>112:E7</t>
-  </si>
-  <si>
-    <t>113:F7</t>
-  </si>
-  <si>
-    <t>114:F#7</t>
-  </si>
-  <si>
-    <t>115:G7</t>
-  </si>
-  <si>
-    <t>116:G#7</t>
-  </si>
-  <si>
-    <t>117:A7</t>
-  </si>
-  <si>
-    <t>118:A#7</t>
-  </si>
-  <si>
-    <t>119:B7</t>
-  </si>
-  <si>
-    <t>120:C8</t>
-  </si>
-  <si>
-    <t>121:C#8</t>
-  </si>
-  <si>
-    <t>122:D8</t>
-  </si>
-  <si>
-    <t>123:D#8</t>
-  </si>
-  <si>
-    <t>124:E8</t>
-  </si>
-  <si>
-    <t>125:F8</t>
-  </si>
-  <si>
-    <t>126:F#8</t>
-  </si>
-  <si>
-    <t>127:G8</t>
-  </si>
-  <si>
     <t>Direction</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -538,6 +154,390 @@
   </si>
   <si>
     <t>Brush</t>
+  </si>
+  <si>
+    <t>C-2 (0)</t>
+  </si>
+  <si>
+    <t>C#-2 (1)</t>
+  </si>
+  <si>
+    <t>D-2 (2)</t>
+  </si>
+  <si>
+    <t>D#-2 (3)</t>
+  </si>
+  <si>
+    <t>E-2 (4)</t>
+  </si>
+  <si>
+    <t>F-2 (5)</t>
+  </si>
+  <si>
+    <t>F#-2 (6)</t>
+  </si>
+  <si>
+    <t>G-2 (7)</t>
+  </si>
+  <si>
+    <t>G#-2 (8)</t>
+  </si>
+  <si>
+    <t>A-2 (9)</t>
+  </si>
+  <si>
+    <t>A#-2 (10)</t>
+  </si>
+  <si>
+    <t>B-2 (11)</t>
+  </si>
+  <si>
+    <t>C-1 (12)</t>
+  </si>
+  <si>
+    <t>C#-1 (13)</t>
+  </si>
+  <si>
+    <t>D-1 (14)</t>
+  </si>
+  <si>
+    <t>D#-1 (15)</t>
+  </si>
+  <si>
+    <t>E-1 (16)</t>
+  </si>
+  <si>
+    <t>F-1 (17)</t>
+  </si>
+  <si>
+    <t>F#-1 (18)</t>
+  </si>
+  <si>
+    <t>G-1 (19)</t>
+  </si>
+  <si>
+    <t>G#-1 (20)</t>
+  </si>
+  <si>
+    <t>A-1 (21)</t>
+  </si>
+  <si>
+    <t>A#-1 (22)</t>
+  </si>
+  <si>
+    <t>B-1 (23)</t>
+  </si>
+  <si>
+    <t>C0 (24)</t>
+  </si>
+  <si>
+    <t>C#0 (25)</t>
+  </si>
+  <si>
+    <t>D0 (26)</t>
+  </si>
+  <si>
+    <t>D#0 (27)</t>
+  </si>
+  <si>
+    <t>E0 (28)</t>
+  </si>
+  <si>
+    <t>F0 (29)</t>
+  </si>
+  <si>
+    <t>F#0 (30)</t>
+  </si>
+  <si>
+    <t>G0 (31)</t>
+  </si>
+  <si>
+    <t>G#0 (32)</t>
+  </si>
+  <si>
+    <t>A0 (33)</t>
+  </si>
+  <si>
+    <t>A#0 (34)</t>
+  </si>
+  <si>
+    <t>B0 (35)</t>
+  </si>
+  <si>
+    <t>C1 (36)</t>
+  </si>
+  <si>
+    <t>C#1 (37)</t>
+  </si>
+  <si>
+    <t>D1 (38)</t>
+  </si>
+  <si>
+    <t>D#1 (39)</t>
+  </si>
+  <si>
+    <t>E1 (40)</t>
+  </si>
+  <si>
+    <t>F1 (41)</t>
+  </si>
+  <si>
+    <t>F#1 (42)</t>
+  </si>
+  <si>
+    <t>G1 (43)</t>
+  </si>
+  <si>
+    <t>G#1 (44)</t>
+  </si>
+  <si>
+    <t>A1 (45)</t>
+  </si>
+  <si>
+    <t>A#1 (46)</t>
+  </si>
+  <si>
+    <t>B1 (47)</t>
+  </si>
+  <si>
+    <t>C2 (48)</t>
+  </si>
+  <si>
+    <t>C#2 (49)</t>
+  </si>
+  <si>
+    <t>D2 (50)</t>
+  </si>
+  <si>
+    <t>D#2 (51)</t>
+  </si>
+  <si>
+    <t>E2 (52)</t>
+  </si>
+  <si>
+    <t>F2 (53)</t>
+  </si>
+  <si>
+    <t>F#2 (54)</t>
+  </si>
+  <si>
+    <t>G2 (55)</t>
+  </si>
+  <si>
+    <t>G#2 (56)</t>
+  </si>
+  <si>
+    <t>A2 (57)</t>
+  </si>
+  <si>
+    <t>A#2 (58)</t>
+  </si>
+  <si>
+    <t>B2 (59)</t>
+  </si>
+  <si>
+    <t>C3 (60)</t>
+  </si>
+  <si>
+    <t>C#3 (61)</t>
+  </si>
+  <si>
+    <t>D3 (62)</t>
+  </si>
+  <si>
+    <t>D#3 (63)</t>
+  </si>
+  <si>
+    <t>E3 (64)</t>
+  </si>
+  <si>
+    <t>F3 (65)</t>
+  </si>
+  <si>
+    <t>F#3 (66)</t>
+  </si>
+  <si>
+    <t>G3 (67)</t>
+  </si>
+  <si>
+    <t>G#3 (68)</t>
+  </si>
+  <si>
+    <t>A3 (69)</t>
+  </si>
+  <si>
+    <t>A#3 (70)</t>
+  </si>
+  <si>
+    <t>B3 (71)</t>
+  </si>
+  <si>
+    <t>C4 (72)</t>
+  </si>
+  <si>
+    <t>C#4 (73)</t>
+  </si>
+  <si>
+    <t>D4 (74)</t>
+  </si>
+  <si>
+    <t>D#4 (75)</t>
+  </si>
+  <si>
+    <t>E4 (76)</t>
+  </si>
+  <si>
+    <t>F4 (77)</t>
+  </si>
+  <si>
+    <t>F#4 (78)</t>
+  </si>
+  <si>
+    <t>G4 (79)</t>
+  </si>
+  <si>
+    <t>G#4 (80)</t>
+  </si>
+  <si>
+    <t>A4 (81)</t>
+  </si>
+  <si>
+    <t>A#4 (82)</t>
+  </si>
+  <si>
+    <t>B4 (83)</t>
+  </si>
+  <si>
+    <t>C5 (84)</t>
+  </si>
+  <si>
+    <t>C#5 (85)</t>
+  </si>
+  <si>
+    <t>D5 (86)</t>
+  </si>
+  <si>
+    <t>D#5 (87)</t>
+  </si>
+  <si>
+    <t>E5 (88)</t>
+  </si>
+  <si>
+    <t>F5 (89)</t>
+  </si>
+  <si>
+    <t>F#5 (90)</t>
+  </si>
+  <si>
+    <t>G5 (91)</t>
+  </si>
+  <si>
+    <t>G#5 (92)</t>
+  </si>
+  <si>
+    <t>A5 (93)</t>
+  </si>
+  <si>
+    <t>A#5 (94)</t>
+  </si>
+  <si>
+    <t>B5 (95)</t>
+  </si>
+  <si>
+    <t>C6 (96)</t>
+  </si>
+  <si>
+    <t>C#6 (97)</t>
+  </si>
+  <si>
+    <t>D6 (98)</t>
+  </si>
+  <si>
+    <t>D#6 (99)</t>
+  </si>
+  <si>
+    <t>E6 (100)</t>
+  </si>
+  <si>
+    <t>F6 (101)</t>
+  </si>
+  <si>
+    <t>F#6 (102)</t>
+  </si>
+  <si>
+    <t>G6 (103)</t>
+  </si>
+  <si>
+    <t>G#6 (104)</t>
+  </si>
+  <si>
+    <t>A6 (105)</t>
+  </si>
+  <si>
+    <t>A#6 (106)</t>
+  </si>
+  <si>
+    <t>B6 (107)</t>
+  </si>
+  <si>
+    <t>C7 (108)</t>
+  </si>
+  <si>
+    <t>C#7 (109)</t>
+  </si>
+  <si>
+    <t>D7 (110)</t>
+  </si>
+  <si>
+    <t>D#7 (111)</t>
+  </si>
+  <si>
+    <t>E7 (112)</t>
+  </si>
+  <si>
+    <t>F7 (113)</t>
+  </si>
+  <si>
+    <t>F#7 (114)</t>
+  </si>
+  <si>
+    <t>G7 (115)</t>
+  </si>
+  <si>
+    <t>G#7 (116)</t>
+  </si>
+  <si>
+    <t>A7 (117)</t>
+  </si>
+  <si>
+    <t>A#7 (118)</t>
+  </si>
+  <si>
+    <t>B7 (119)</t>
+  </si>
+  <si>
+    <t>C8 (120)</t>
+  </si>
+  <si>
+    <t>C#8 (121)</t>
+  </si>
+  <si>
+    <t>D8 (122)</t>
+  </si>
+  <si>
+    <t>D#8 (123)</t>
+  </si>
+  <si>
+    <t>E8 (124)</t>
+  </si>
+  <si>
+    <t>F8 (125)</t>
+  </si>
+  <si>
+    <t>F#8 (126)</t>
+  </si>
+  <si>
+    <t>G8 (127)</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1055,7 @@
       <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1074,13 +1074,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>1</v>
@@ -1089,10 +1089,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>3</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="7" t="s">
-        <v>141</v>
+        <v>13</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
@@ -1115,19 +1115,19 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="F3" s="6">
         <v>120</v>
@@ -1138,19 +1138,19 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="F4" s="6">
         <v>120</v>
@@ -1161,19 +1161,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
-        <v>144</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>144</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="F5" s="6">
         <v>120</v>
@@ -1184,19 +1184,19 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="F6" s="6">
         <v>120</v>
@@ -1207,19 +1207,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>146</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>146</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F7" s="6">
         <v>120</v>
@@ -1230,19 +1230,19 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>147</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>147</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F8" s="6">
         <v>120</v>
@@ -1253,19 +1253,19 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="F9" s="6">
         <v>120</v>
@@ -1276,19 +1276,19 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F10" s="6">
         <v>120</v>
@@ -1299,19 +1299,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="F11" s="6">
         <v>120</v>
@@ -1322,19 +1322,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F12" s="6">
         <v>120</v>
@@ -1345,19 +1345,19 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>152</v>
+        <v>24</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>152</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="F13" s="6">
         <v>120</v>
@@ -1368,19 +1368,19 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F14" s="6">
         <v>120</v>
@@ -1391,19 +1391,19 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6">
         <v>1</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F15" s="6">
         <v>120</v>
@@ -1414,19 +1414,19 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
       <c r="B16" s="6">
         <v>1</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="F16" s="6">
         <v>120</v>
@@ -1437,19 +1437,19 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="B17" s="6">
         <v>1</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="F17" s="6">
         <v>120</v>
@@ -1460,19 +1460,19 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="B18" s="6">
         <v>1</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="F18" s="6">
         <v>120</v>
@@ -1483,19 +1483,19 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F19" s="6">
         <v>120</v>
@@ -1506,19 +1506,19 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F20" s="6">
         <v>120</v>
@@ -1529,19 +1529,19 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
-        <v>160</v>
+        <v>32</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>160</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="F21" s="6">
         <v>120</v>
@@ -1552,19 +1552,19 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>161</v>
+        <v>33</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>161</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="F22" s="6">
         <v>120</v>
@@ -3234,10 +3234,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>135</v>
+        <v>7</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3246,773 +3246,773 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="10" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="10" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="10" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="10" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="10" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="10" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="10" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="10" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B17" s="8"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="10" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="10" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="10" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B22" s="8"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="10" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B23" s="8"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="10" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B24" s="8"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="10" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B25" s="8"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="10" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B26" s="8"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="10" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="B27" s="8"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="10" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B28" s="8"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="10" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="10" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B30" s="8"/>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="10" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B31" s="8"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="10" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B32" s="8"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="10" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B33" s="8"/>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="10" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B34" s="8"/>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="10" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B35" s="8"/>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="10" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B36" s="8"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="10" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B37" s="8"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="10" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="B38" s="8"/>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="10" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B39" s="8"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="10" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B40" s="8"/>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="10" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B41" s="8"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="10" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B42" s="8"/>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="10" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="B43" s="8"/>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="10" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B44" s="8"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="10" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B45" s="8"/>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="10" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="10" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="10" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="10" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B49" s="8"/>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="10" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="10" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B51" s="8"/>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="10" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="B52" s="8"/>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="10" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="B53" s="8"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="10" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="10" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="B55" s="8"/>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="10" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B56" s="8"/>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="10" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B57" s="8"/>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="10" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B58" s="8"/>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="10" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B59" s="8"/>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="10" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="B60" s="8"/>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="10" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B61" s="8"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="10" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="B62" s="8"/>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="10" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B63" s="8"/>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="10" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B64" s="8"/>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="10" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B65" s="8"/>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="10" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="B66" s="8"/>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="10" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="B67" s="8"/>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="10" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="B68" s="8"/>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="10" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="B69" s="8"/>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="10" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="B70" s="8"/>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="10" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B71" s="8"/>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="10" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B72" s="8"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="10" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B73" s="8"/>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="10" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="B74" s="8"/>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="10" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="B75" s="8"/>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="10" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B76" s="8"/>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="10" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="B77" s="8"/>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="10" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="B78" s="8"/>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="10" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="B79" s="8"/>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="10" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="B80" s="8"/>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="10" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="B81" s="8"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="10" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B82" s="8"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="10" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="B83" s="8"/>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="10" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="B84" s="8"/>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="10" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B85" s="8"/>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="10" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="B86" s="8"/>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="10" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="B87" s="8"/>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="10" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B88" s="8"/>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="10" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="B89" s="8"/>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="10" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="B90" s="8"/>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="10" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="B91" s="8"/>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="10" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B92" s="8"/>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="10" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="B93" s="8"/>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="10" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="B94" s="8"/>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="10" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="B95" s="8"/>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="10" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="B96" s="8"/>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="10" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="B97" s="8"/>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="10" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="B98" s="8"/>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="10" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="B99" s="8"/>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="10" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="B100" s="8"/>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="10" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="B101" s="8"/>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="10" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B102" s="8"/>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="10" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="B103" s="8"/>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="10" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="B104" s="8"/>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="10" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="B105" s="8"/>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="10" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="B106" s="8"/>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="10" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="B107" s="8"/>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="10" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B108" s="8"/>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="10" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="B109" s="8"/>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="10" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="B110" s="8"/>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="10" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="B111" s="8"/>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="10" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B112" s="8"/>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="10" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="B113" s="8"/>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="10" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="B114" s="8"/>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="10" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="B115" s="8"/>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="10" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="B116" s="8"/>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="10" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="B117" s="8"/>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="10" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="B118" s="8"/>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="10" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="B119" s="8"/>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="10" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="B120" s="8"/>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="10" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="B121" s="8"/>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="10" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="B122" s="8"/>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="10" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="B123" s="8"/>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="10" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="B124" s="8"/>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="10" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B125" s="8"/>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="10" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="B126" s="8"/>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="10" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="B127" s="8"/>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="10" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="B128" s="8"/>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="10" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="B129" s="8"/>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="10" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>